<commit_message>
Adicionado o filtro para pesquisa com todos os campos de despesa
</commit_message>
<xml_diff>
--- a/routes/filesXLSX/write.xlsx
+++ b/routes/filesXLSX/write.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t xml:space="preserve">gfvb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aniver</t>
   </si>
 </sst>
 </file>
@@ -158,13 +164,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.8"/>
   </cols>
@@ -237,6 +243,20 @@
       </c>
       <c r="D5" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>43893</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>